<commit_message>
teste de captura de erros
</commit_message>
<xml_diff>
--- a/informacao_municipio.xlsx
+++ b/informacao_municipio.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2483" uniqueCount="977">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2483" uniqueCount="978">
   <si>
     <t>Cod_IBGE</t>
   </si>
@@ -2947,6 +2947,9 @@
   </si>
   <si>
     <t>2238.85</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
 </sst>
 </file>
@@ -3295,8 +3298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X225"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:X225"/>
+    <sheetView tabSelected="1" topLeftCell="B199" workbookViewId="0">
+      <selection activeCell="X225" sqref="X225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19955,7 +19958,7 @@
         <v>976</v>
       </c>
       <c r="X225" s="1" t="s">
-        <v>780</v>
+        <v>977</v>
       </c>
     </row>
   </sheetData>

</xml_diff>